<commit_message>
1. Split the Skills from Equipment into its own Entity; 2. Created the new Repo Interface; 3. Updated Excel Service to allow upload of SkillList; 4) Updated Excel and GET Controllers
</commit_message>
<xml_diff>
--- a/src/main/resources/EquipmentData.xlsx
+++ b/src/main/resources/EquipmentData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OO39XP\workprojects\MonsterHunterEquipmentSet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCB737F-C250-44FD-B623-02A48F37E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C638F08-837A-4202-9252-CC48433D3D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DF2D5C21-E555-49DE-BC7B-597438759B63}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{DF2D5C21-E555-49DE-BC7B-597438759B63}"/>
   </bookViews>
   <sheets>
     <sheet name="EquipmentList" sheetId="1" r:id="rId1"/>
+    <sheet name="SkillList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -47,12 +48,6 @@
     <t>slots</t>
   </si>
   <si>
-    <t>skill</t>
-  </si>
-  <si>
-    <t>skillLevel</t>
-  </si>
-  <si>
     <t>defensePoints</t>
   </si>
   <si>
@@ -68,34 +63,67 @@
     <t>dragonRes</t>
   </si>
   <si>
-    <t>Rathian Helm</t>
-  </si>
-  <si>
-    <t>Rathian Mail</t>
-  </si>
-  <si>
-    <t>Rathian Braces</t>
-  </si>
-  <si>
-    <t>Rathian Coil</t>
-  </si>
-  <si>
-    <t>Rathian Greaves</t>
-  </si>
-  <si>
-    <t>Helm</t>
+    <t>waterRes</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Lv</t>
+  </si>
+  <si>
+    <t>Rathalos Helm S</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Rathalos Mail S</t>
   </si>
   <si>
     <t>Chest</t>
   </si>
   <si>
+    <t>Rathalos Braces S</t>
+  </si>
+  <si>
     <t>Arms</t>
   </si>
   <si>
+    <t>Rathalos Coil S</t>
+  </si>
+  <si>
     <t>Waist</t>
   </si>
   <si>
-    <t>Leg</t>
+    <t>Rathalos Greaves S</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Rathian Helm S</t>
+  </si>
+  <si>
+    <t>Rathian Mail S</t>
+  </si>
+  <si>
+    <t>Rathian Braces S</t>
+  </si>
+  <si>
+    <t>Rathian Coil S</t>
+  </si>
+  <si>
+    <t>Rathian Greaves S</t>
+  </si>
+  <si>
+    <t>Attack Boost</t>
+  </si>
+  <si>
+    <t>Partbreaker</t>
+  </si>
+  <si>
+    <t>Windproof</t>
   </si>
   <si>
     <t>Blight Resistance</t>
@@ -104,22 +132,40 @@
     <t>Recovery Up</t>
   </si>
   <si>
+    <t>Botanist</t>
+  </si>
+  <si>
+    <t>Wide-Range</t>
+  </si>
+  <si>
     <t>Free Meal</t>
-  </si>
-  <si>
-    <t>waterRes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,8 +188,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,235 +519,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B130ADEB-862B-4664-8864-DDB736CDF694}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="1.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>62</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>62</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>62</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>62</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>62</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>52</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>52</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>52</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>52</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>52</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EA9B8D-E0F8-4979-9322-5141D57F6226}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>-2</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>-2</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>22</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>-2</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>22</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>-2</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>22</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>-2</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>-3</v>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>